<commit_message>
minor edits to files to identify columns for joining
</commit_message>
<xml_diff>
--- a/data/juvenile/GSI/PID20240039(2)_WCVI_FTF(22-23)_sc578_2024-07-11_NF_JB -- 2023 SJ purse seine part 2.xlsx
+++ b/data/juvenile/GSI/PID20240039(2)_WCVI_FTF(22-23)_sc578_2024-07-11_NF_JB -- 2023 SJ purse seine part 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\data\juvenile\GSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76923E9-7D1B-4450-A298-B936A231AC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028F5C86-0607-4E97-B223-D7077C8671A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="842" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="842" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData" sheetId="4" r:id="rId1"/>
@@ -10596,7 +10596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E390"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="E302" sqref="E302"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19782,8 +19784,8 @@
   </sheetPr>
   <dimension ref="A1:T166"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19795,16 +19797,16 @@
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -19822,52 +19824,52 @@
       <c r="D1" s="9" t="s">
         <v>822</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>824</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>825</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>826</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="10" t="s">
         <v>827</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>828</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>829</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="10" t="s">
         <v>830</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>831</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="10" t="s">
         <v>832</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="10" t="s">
         <v>833</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="10" t="s">
         <v>834</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="10" t="s">
         <v>835</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="10" t="s">
         <v>838</v>
       </c>
     </row>
@@ -28002,7 +28004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31577,7 +31579,9 @@
   </sheetPr>
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -43229,6 +43233,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="60fc0c19-d104-4386-a9bb-40357a5c460e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="690b556a-b63a-4585-bf5e-b4785f5b05a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056D8E9F490D9BE48AAED4C23D289B6D2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b26ad163c7507b5e93943df7f3881b59">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="690b556a-b63a-4585-bf5e-b4785f5b05a4" xmlns:ns3="60fc0c19-d104-4386-a9bb-40357a5c460e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98e67ad6160fe202e3b53629db83b726" ns2:_="" ns3:_="">
     <xsd:import namespace="690b556a-b63a-4585-bf5e-b4785f5b05a4"/>
@@ -43477,27 +43501,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3393B404-4ED4-498E-ABC4-E78E4188FA1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="60fc0c19-d104-4386-a9bb-40357a5c460e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="690b556a-b63a-4585-bf5e-b4785f5b05a4"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="60fc0c19-d104-4386-a9bb-40357a5c460e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="690b556a-b63a-4585-bf5e-b4785f5b05a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E76CF1-1503-457C-BD28-BCCDDCA7145E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F6E7708-1F1E-4452-AF59-51AE3D3F6B09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43514,29 +43543,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0E76CF1-1503-457C-BD28-BCCDDCA7145E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3393B404-4ED4-498E-ABC4-E78E4188FA1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="60fc0c19-d104-4386-a9bb-40357a5c460e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="690b556a-b63a-4585-bf5e-b4785f5b05a4"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>